<commit_message>
refactor, success importing and run rebuild
</commit_message>
<xml_diff>
--- a/storage/app/import/master-materials-tools-cn.xlsx
+++ b/storage/app/import/master-materials-tools-cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\MeMFIS\storage\app\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4875C06D-ACCF-4777-9544-D1DF70AB85AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0E6500-C390-4E49-96F5-A5B8E1EBF21C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8490" yWindow="1665" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="76">
   <si>
     <t>Material</t>
   </si>
@@ -135,9 +135,6 @@
     <t>35-13328-0801</t>
   </si>
   <si>
-    <t>Solvent Z-23.138</t>
-  </si>
-  <si>
     <t>Emulsion Cleaner  Z-23.212</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Grease</t>
   </si>
   <si>
-    <t>Cleaning Solvent</t>
-  </si>
-  <si>
     <t>Scotch Brite</t>
   </si>
   <si>
@@ -232,6 +226,33 @@
   </si>
   <si>
     <t>Access Platform 2.5 M High</t>
+  </si>
+  <si>
+    <t>RAW-PL-PUTIH</t>
+  </si>
+  <si>
+    <t>RAW-NR094-A</t>
+  </si>
+  <si>
+    <t>Lint Free Cloth</t>
+  </si>
+  <si>
+    <t>Cleaning Solvent Z-23.138</t>
+  </si>
+  <si>
+    <t>35-11392-0403-A</t>
+  </si>
+  <si>
+    <t>35-13328-0401-A</t>
+  </si>
+  <si>
+    <t>28-0-2243-MZ-A</t>
+  </si>
+  <si>
+    <t>28-0-2243-MZ-B</t>
+  </si>
+  <si>
+    <t>28-0-2243-MZ-C</t>
   </si>
 </sst>
 </file>
@@ -805,18 +826,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="256" max="256" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="257" max="257" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="264" max="264" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -1036,40 +1060,44 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="G3" s="8"/>
       <c r="H3" s="8" t="s">
         <v>10</v>
       </c>
@@ -1079,7 +1107,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>20</v>
@@ -1087,39 +1115,43 @@
       <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E4" s="8"/>
       <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="G5" s="8"/>
       <c r="H5" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>20</v>
@@ -1127,9 +1159,11 @@
       <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E6" s="8"/>
       <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1139,7 +1173,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>20</v>
@@ -1147,9 +1181,11 @@
       <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E7" s="8"/>
       <c r="F7" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
         <v>10</v>
       </c>
@@ -1159,7 +1195,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>20</v>
@@ -1167,9 +1203,11 @@
       <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E8" s="8"/>
       <c r="F8" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
         <v>10</v>
       </c>
@@ -1179,7 +1217,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>20</v>
@@ -1187,9 +1225,11 @@
       <c r="D9" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E9" s="8"/>
       <c r="F9" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1239,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>20</v>
@@ -1207,9 +1247,11 @@
       <c r="D10" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E10" s="8"/>
       <c r="F10" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1219,7 +1261,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>20</v>
@@ -1227,9 +1269,11 @@
       <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E11" s="8"/>
       <c r="F11" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
         <v>10</v>
       </c>
@@ -1239,7 +1283,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>20</v>
@@ -1247,9 +1291,11 @@
       <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E12" s="8"/>
       <c r="F12" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
         <v>10</v>
       </c>
@@ -1259,7 +1305,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>20</v>
@@ -1267,9 +1313,11 @@
       <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E13" s="8"/>
       <c r="F13" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
         <v>10</v>
       </c>
@@ -1279,7 +1327,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>20</v>
@@ -1287,9 +1335,11 @@
       <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E14" s="8"/>
       <c r="F14" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G14" s="8"/>
       <c r="H14" s="8" t="s">
         <v>10</v>
       </c>
@@ -1299,7 +1349,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>20</v>
@@ -1307,19 +1357,21 @@
       <c r="D15" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E15" s="8"/>
       <c r="F15" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G15" s="8"/>
       <c r="H15" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>20</v>
@@ -1327,9 +1379,11 @@
       <c r="D16" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E16" s="8"/>
       <c r="F16" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G16" s="8"/>
       <c r="H16" s="8" t="s">
         <v>10</v>
       </c>
@@ -1339,7 +1393,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>20</v>
@@ -1347,19 +1401,21 @@
       <c r="D17" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E17" s="8"/>
       <c r="F17" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>20</v>
@@ -1367,9 +1423,11 @@
       <c r="D18" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G18" s="8"/>
       <c r="H18" s="8" t="s">
         <v>10</v>
       </c>
@@ -1379,7 +1437,7 @@
         <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>20</v>
@@ -1387,9 +1445,11 @@
       <c r="D19" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E19" s="8"/>
       <c r="F19" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
         <v>10</v>
       </c>
@@ -1399,7 +1459,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>20</v>
@@ -1407,9 +1467,11 @@
       <c r="D20" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E20" s="8"/>
       <c r="F20" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G20" s="8"/>
       <c r="H20" s="8" t="s">
         <v>10</v>
       </c>
@@ -1419,7 +1481,7 @@
         <v>35</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>20</v>
@@ -1427,9 +1489,11 @@
       <c r="D21" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E21" s="8"/>
       <c r="F21" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G21" s="8"/>
       <c r="H21" s="8" t="s">
         <v>10</v>
       </c>
@@ -1439,7 +1503,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>20</v>
@@ -1447,9 +1511,11 @@
       <c r="D22" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E22" s="8"/>
       <c r="F22" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G22" s="8"/>
       <c r="H22" s="8" t="s">
         <v>10</v>
       </c>
@@ -1459,7 +1525,7 @@
         <v>42019691</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>8</v>
@@ -1467,29 +1533,33 @@
       <c r="D23" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E23" s="8"/>
       <c r="F23" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G23" s="8"/>
       <c r="H23" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="47.25">
+    <row r="24" spans="1:8" ht="31.5">
       <c r="A24" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E24" s="8"/>
       <c r="F24" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G24" s="8"/>
       <c r="H24" s="8" t="s">
         <v>10</v>
       </c>
@@ -1499,7 +1569,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>8</v>
@@ -1507,19 +1577,21 @@
       <c r="D25" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E25" s="8"/>
       <c r="F25" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G25" s="8"/>
       <c r="H25" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="31.5">
+    <row r="26" spans="1:8" ht="15.75">
       <c r="A26" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>8</v>
@@ -1527,9 +1599,11 @@
       <c r="D26" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E26" s="8"/>
       <c r="F26" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G26" s="8"/>
       <c r="H26" s="8" t="s">
         <v>10</v>
       </c>
@@ -1539,7 +1613,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>8</v>
@@ -1547,69 +1621,77 @@
       <c r="D27" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E27" s="8"/>
       <c r="F27" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G27" s="8"/>
       <c r="H27" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75">
       <c r="A28" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75">
+      <c r="A29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75">
+      <c r="A30" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="31.5">
-      <c r="A29" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="47.25">
-      <c r="A30" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="C30" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E30" s="8"/>
       <c r="F30" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G30" s="8"/>
       <c r="H30" s="8" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1701,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>8</v>
@@ -1627,19 +1709,21 @@
       <c r="D31" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G31" s="8"/>
       <c r="H31" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75">
       <c r="A32" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>8</v>
@@ -1647,19 +1731,21 @@
       <c r="D32" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E32" s="8"/>
       <c r="F32" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G32" s="8"/>
       <c r="H32" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="25.5">
       <c r="A33" s="7" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>8</v>
@@ -1667,19 +1753,21 @@
       <c r="D33" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E33" s="8"/>
       <c r="F33" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G33" s="8"/>
       <c r="H33" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75">
       <c r="A34" s="7" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>8</v>
@@ -1687,19 +1775,21 @@
       <c r="D34" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E34" s="8"/>
       <c r="F34" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G34" s="8"/>
       <c r="H34" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75">
       <c r="A35" s="7" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>8</v>
@@ -1707,15 +1797,14 @@
       <c r="D35" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E35" s="8"/>
       <c r="F35" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>